<commit_message>
- updated parts list
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="84">
   <si>
     <t>Parts ideas</t>
   </si>
@@ -94,6 +94,183 @@
   </si>
   <si>
     <t>2-pole audio connector</t>
+  </si>
+  <si>
+    <t>DC power supply</t>
+  </si>
+  <si>
+    <t>mains AC adaptor</t>
+  </si>
+  <si>
+    <t>2.5mm jack</t>
+  </si>
+  <si>
+    <t>Mnfctr</t>
+  </si>
+  <si>
+    <t>Multicomp</t>
+  </si>
+  <si>
+    <t>MCPLG12V10WUK</t>
+  </si>
+  <si>
+    <t>Mnfctr. part no.</t>
+  </si>
+  <si>
+    <t>12V, 10W output</t>
+  </si>
+  <si>
+    <t>Lumberg</t>
+  </si>
+  <si>
+    <t>KLS 2</t>
+  </si>
+  <si>
+    <t>Pro Signal</t>
+  </si>
+  <si>
+    <t>MJ-164H</t>
+  </si>
+  <si>
+    <t>MJ-15SR</t>
+  </si>
+  <si>
+    <t>MP-122M</t>
+  </si>
+  <si>
+    <t>25.413.1</t>
+  </si>
+  <si>
+    <t>25.413.2</t>
+  </si>
+  <si>
+    <t>24.247.1</t>
+  </si>
+  <si>
+    <t>24.247.2</t>
+  </si>
+  <si>
+    <t>On-off (rocker) switch</t>
+  </si>
+  <si>
+    <t>SPST</t>
+  </si>
+  <si>
+    <t>250V, 16A max, illuminated</t>
+  </si>
+  <si>
+    <t>MC34231-091-72</t>
+  </si>
+  <si>
+    <t>MC34224-071-1501</t>
+  </si>
+  <si>
+    <t>20A, non-illuminated, black/red</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>Rotor</t>
+  </si>
+  <si>
+    <t>BI Technologies</t>
+  </si>
+  <si>
+    <t>P160KNP-0QC20B10K</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>249BBHS0XB25103KA</t>
+  </si>
+  <si>
+    <t>10k, 1W, +-10%</t>
+  </si>
+  <si>
+    <t>10k, 200mW, +-20%</t>
+  </si>
+  <si>
+    <t>13-25</t>
+  </si>
+  <si>
+    <t>BNC panel mount</t>
+  </si>
+  <si>
+    <t>50 Ohm</t>
+  </si>
+  <si>
+    <t>brass, &lt;11GHz</t>
+  </si>
+  <si>
+    <t>Test point</t>
+  </si>
+  <si>
+    <t>thru-hole</t>
+  </si>
+  <si>
+    <t>1mm diamter</t>
+  </si>
+  <si>
+    <t>TEST-3</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>this or 249BBHS0XB25103KA</t>
+  </si>
+  <si>
+    <t>this or P160KNP-0QC20B10K</t>
+  </si>
+  <si>
+    <t>Keystone</t>
+  </si>
+  <si>
+    <t>pack of 100, alt. to TEST-3</t>
+  </si>
+  <si>
+    <t>for panel mounting</t>
+  </si>
+  <si>
+    <t>pack of 100, alt. to 1035</t>
+  </si>
+  <si>
+    <t>5k, 1W, +-10%</t>
+  </si>
+  <si>
+    <t>purpose</t>
+  </si>
+  <si>
+    <t>V_offset</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>249BBHS0XB25502KA</t>
+  </si>
+  <si>
+    <t>RG_select</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>SPDT</t>
+  </si>
+  <si>
+    <t>1MS1T1B5M1QE</t>
+  </si>
+  <si>
+    <t>max 5A</t>
+  </si>
+  <si>
+    <t>panel mount, On-On</t>
+  </si>
+  <si>
+    <t>not needed if power supply used</t>
   </si>
 </sst>
 </file>
@@ -605,7 +782,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -616,6 +793,8 @@
     <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -938,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -950,13 +1129,14 @@
     <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -967,7 +1147,7 @@
         <v>42671</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -979,8 +1159,11 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -994,22 +1177,34 @@
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1023,21 +1218,30 @@
         <v>19</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
         <v>0.5</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>1698951</v>
       </c>
-      <c r="I5" s="3">
-        <f>E5*F5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="3">
+        <f>F5*G5</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1051,21 +1255,30 @@
         <v>19</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
         <v>0.5</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>1698950</v>
       </c>
-      <c r="I6" s="3">
-        <f t="shared" ref="I6:I12" si="0">E6*F6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" ref="L6:L22" si="0">F6*G6</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1079,21 +1292,30 @@
         <v>19</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
         <v>1.35</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <v>1698964</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1107,21 +1329,30 @@
         <v>19</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
         <v>1.35</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>1698963</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -1135,21 +1366,33 @@
         <v>17</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
         <v>0.5</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <v>1737249</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+      <c r="M9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1163,21 +1406,30 @@
         <v>17</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="3">
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="3">
         <v>0.9</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <v>1737252</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
@@ -1191,21 +1443,30 @@
         <v>17</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="3">
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3">
         <v>0.73</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <v>1243261</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1219,32 +1480,420 @@
         <v>17</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1.24</v>
+      </c>
+      <c r="H12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>1267394</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>1827445</v>
+      </c>
+      <c r="J13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14">
+        <v>1454386</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <v>1454382</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="0"/>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16">
+        <v>1760793</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="M16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3">
+        <v>6.94</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17">
+        <v>9609245</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K17" t="s">
+        <v>54</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" si="0"/>
+        <v>6.94</v>
+      </c>
+      <c r="M17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1.67</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18">
+        <v>1169699</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K18" t="s">
+        <v>57</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" si="0"/>
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1.41</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19">
+        <v>1702006</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" t="s">
+        <v>64</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="0"/>
+        <v>1.41</v>
+      </c>
+      <c r="M19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>13.7</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20">
+        <v>2112492</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K20" s="9">
+        <v>1035</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="0"/>
+        <v>13.7</v>
+      </c>
+      <c r="M20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" s="3">
+        <v>6.33</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21">
+        <v>9609237</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="K21" t="s">
+        <v>76</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="0"/>
+        <v>6.33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22">
+        <v>9473378</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1"/>
-    <hyperlink ref="G6" r:id="rId2"/>
-    <hyperlink ref="G7" r:id="rId3"/>
-    <hyperlink ref="G8" r:id="rId4"/>
-    <hyperlink ref="G9" r:id="rId5" location="techDocsHook"/>
-    <hyperlink ref="G10" r:id="rId6"/>
-    <hyperlink ref="G11" r:id="rId7"/>
-    <hyperlink ref="G12" r:id="rId8"/>
+    <hyperlink ref="H5" r:id="rId1"/>
+    <hyperlink ref="H6" r:id="rId2"/>
+    <hyperlink ref="H7" r:id="rId3"/>
+    <hyperlink ref="H8" r:id="rId4"/>
+    <hyperlink ref="H9" r:id="rId5" location="techDocsHook"/>
+    <hyperlink ref="H10" r:id="rId6"/>
+    <hyperlink ref="H11" r:id="rId7"/>
+    <hyperlink ref="H12" r:id="rId8"/>
+    <hyperlink ref="H13" r:id="rId9"/>
+    <hyperlink ref="H14" r:id="rId10"/>
+    <hyperlink ref="H15" r:id="rId11"/>
+    <hyperlink ref="H16" r:id="rId12"/>
+    <hyperlink ref="H17" r:id="rId13"/>
+    <hyperlink ref="H18" r:id="rId14"/>
+    <hyperlink ref="H19" r:id="rId15"/>
+    <hyperlink ref="H20" r:id="rId16"/>
+    <hyperlink ref="H21" r:id="rId17"/>
+    <hyperlink ref="H22" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated box design svg and parts list
</commit_message>
<xml_diff>
--- a/Parts.xlsx
+++ b/Parts.xlsx
@@ -20,17 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="90">
-  <si>
-    <t xml:space="preserve">Parts ideas</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="89">
+  <si>
+    <t xml:space="preserve">Distillation column BOM</t>
   </si>
   <si>
     <t xml:space="preserve">RAS-J</t>
   </si>
   <si>
-    <t xml:space="preserve">Potential parts</t>
-  </si>
-  <si>
     <t xml:space="preserve">Part</t>
   </si>
   <si>
@@ -232,7 +229,7 @@
     <t xml:space="preserve">for panel mounting</t>
   </si>
   <si>
-    <t xml:space="preserve">1mm diamter</t>
+    <t xml:space="preserve">1mm diameter</t>
   </si>
   <si>
     <t xml:space="preserve">TEST-3</t>
@@ -525,22 +522,22 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7091836734694"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="5.58673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.1785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="6.54081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.41836734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0612244897959"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="17.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.55612244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="6.41836734693878"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6.30102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="17.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.44387755102041"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -551,10 +548,8 @@
         <v>42671</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -569,57 +564,57 @@
     </row>
     <row r="4" s="4" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="n">
@@ -629,16 +624,16 @@
         <v>0.5</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I5" s="7" t="n">
         <v>1698951</v>
       </c>
       <c r="J5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="L5" s="5" t="n">
         <f aca="false">F5*G5</f>
@@ -647,16 +642,16 @@
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="n">
@@ -666,16 +661,16 @@
         <v>0.5</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="7" t="n">
         <v>1698950</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L6" s="5" t="n">
         <f aca="false">F6*G6</f>
@@ -684,16 +679,16 @@
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="n">
@@ -703,16 +698,16 @@
         <v>1.35</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I7" s="7" t="n">
         <v>1698964</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7" s="5" t="n">
         <f aca="false">F7*G7</f>
@@ -721,16 +716,16 @@
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="n">
@@ -740,16 +735,16 @@
         <v>1.35</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" s="7" t="n">
         <v>1698963</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L8" s="5" t="n">
         <f aca="false">F8*G8</f>
@@ -758,16 +753,16 @@
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="n">
@@ -777,37 +772,37 @@
         <v>0.5</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I9" s="7" t="n">
         <v>1737249</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L9" s="5" t="n">
         <f aca="false">F9*G9</f>
         <v>0.5</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="n">
@@ -817,16 +812,16 @@
         <v>0.9</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10" s="7" t="n">
         <v>1737252</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L10" s="5" t="n">
         <f aca="false">F10*G10</f>
@@ -835,16 +830,16 @@
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="n">
@@ -854,16 +849,16 @@
         <v>0.73</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I11" s="7" t="n">
         <v>1243261</v>
       </c>
       <c r="J11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>38</v>
       </c>
       <c r="L11" s="5" t="n">
         <f aca="false">F11*G11</f>
@@ -872,16 +867,16 @@
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="n">
@@ -891,16 +886,16 @@
         <v>1.24</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I12" s="7" t="n">
         <v>1267394</v>
       </c>
       <c r="J12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>40</v>
       </c>
       <c r="L12" s="5" t="n">
         <f aca="false">F12*G12</f>
@@ -909,16 +904,16 @@
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="n">
@@ -928,16 +923,16 @@
         <v>7.5</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>1827445</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L13" s="5" t="n">
         <f aca="false">F13*G13</f>
@@ -946,13 +941,13 @@
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>1</v>
@@ -961,16 +956,16 @@
         <v>1.16</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>1454386</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L14" s="5" t="n">
         <f aca="false">F14*G14</f>
@@ -979,13 +974,13 @@
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="3" t="n">
         <v>1</v>
@@ -994,16 +989,16 @@
         <v>0.64</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>1454382</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L15" s="5" t="n">
         <f aca="false">F15*G15</f>
@@ -1012,16 +1007,16 @@
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="E16" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>0</v>
@@ -1030,37 +1025,37 @@
         <v>0.61</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>1760793</v>
       </c>
       <c r="J16" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="K16" s="0" t="s">
         <v>56</v>
-      </c>
-      <c r="K16" s="0" t="s">
-        <v>57</v>
       </c>
       <c r="L16" s="5" t="n">
         <f aca="false">F16*G16</f>
         <v>0</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="C17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F17" s="3" t="n">
         <v>1</v>
@@ -1069,37 +1064,37 @@
         <v>6.94</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>9609245</v>
       </c>
       <c r="J17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K17" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>61</v>
       </c>
       <c r="L17" s="5" t="n">
         <f aca="false">F17*G17</f>
         <v>6.94</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="0" t="n">
@@ -1109,16 +1104,16 @@
         <v>1.67</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>1169699</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L18" s="5" t="n">
         <f aca="false">F18*G18</f>
@@ -1127,16 +1122,16 @@
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="0" t="n">
@@ -1146,34 +1141,34 @@
         <v>1.41</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>1702006</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L19" s="5" t="n">
         <f aca="false">F19*G19</f>
         <v>1.41</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="F20" s="0" t="n">
         <v>0</v>
@@ -1182,13 +1177,13 @@
         <v>13.7</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>2112492</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K20" s="8" t="n">
         <v>1035</v>
@@ -1198,21 +1193,21 @@
         <v>0</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="F21" s="0" t="n">
         <v>1</v>
@@ -1221,16 +1216,16 @@
         <v>6.33</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>9609237</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L21" s="5" t="n">
         <f aca="false">F21*G21</f>
@@ -1239,19 +1234,19 @@
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="E22" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>82</v>
       </c>
       <c r="F22" s="0" t="n">
         <v>1</v>
@@ -1260,16 +1255,16 @@
         <v>1.4</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>9473378</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L22" s="5" t="n">
         <f aca="false">F22*G22</f>
@@ -1278,13 +1273,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="C23" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="F23" s="0" t="n">
         <v>1</v>
@@ -1293,16 +1288,16 @@
         <v>5.56</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I23" s="3" t="n">
         <v>2294665</v>
       </c>
       <c r="J23" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="K23" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="L23" s="5" t="n">
         <f aca="false">F23*G23</f>
@@ -1311,7 +1306,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K27" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L27" s="0" t="n">
         <f aca="false">SUM(L5:L24)</f>

</xml_diff>